<commit_message>
Adicion de paginas nuevas, cambio de imagenes
El login esta finalizado
</commit_message>
<xml_diff>
--- a/Casos de Prueba y Manual/CasosDePrueba.xlsx
+++ b/Casos de Prueba y Manual/CasosDePrueba.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t xml:space="preserve">Nombre de Caso </t>
   </si>
@@ -82,6 +82,105 @@
   </si>
   <si>
     <t>Nivel De Aplicación(porcentaje)</t>
+  </si>
+  <si>
+    <t>Extracción de informacion mediante JavaScript</t>
+  </si>
+  <si>
+    <t>Uso de JavaScript para 
+extraer información de 
+inputs para mandar PHP</t>
+  </si>
+  <si>
+    <t>Extracción de información
+correcta en JavaScript. Print
+con esa información</t>
+  </si>
+  <si>
+    <t>Información erronea, por 
+ejemplo, el value de un boton.</t>
+  </si>
+  <si>
+    <t>Información correcta, si agarro 
+los inputs correctamente.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formateo de arreglos a JSON </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uso de formato de JSON 
+como formato comun para
+intercambio de 
+información. </t>
+  </si>
+  <si>
+    <t>Arreglo JSON visible en PHP.</t>
+  </si>
+  <si>
+    <t>Extracción de información
+correcta en JavaScript. Print
+con esa información.</t>
+  </si>
+  <si>
+    <t>Fallo en función de conversión,
+no se paso la información
+correctamente entre JavaScript
+y PHP.</t>
+  </si>
+  <si>
+    <t>Información recibida
+correctamente por PHP.</t>
+  </si>
+  <si>
+    <t>Pruebas de Procedimientos Almacenados
+USUARIO, PHONE, EMAIL, PERSON</t>
+  </si>
+  <si>
+    <t>Se prueban los paquetes y 
+sus procedimientos y 
+funciones respectivas
+dentro de la base de datos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inserts a tablas, y valores
+correctos de returns. </t>
+  </si>
+  <si>
+    <t>Errores de compilación, falta de
+información correcta.</t>
+  </si>
+  <si>
+    <t>Despliegue de información
+correcta a output. Además, se 
+insertaron los datos
+correctamente dentro de las
+tablas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conexion entre interfaz gráfica, </t>
+  </si>
+  <si>
+    <t>Después de haber conectado
+e interlazado las diferentes
+partes de la aplicación, se
+prueban en conjunto
+para ver como 
+interactuan con si mismas.</t>
+  </si>
+  <si>
+    <t>Inserción de datos a la base,
+despliegue de mensajes de
+error o éxito en la interfaz, 
+transmisión de información por
+medio de MVC.</t>
+  </si>
+  <si>
+    <t>Se inserto la información 
+correctamente. En caso de
+excepciones con lo que se debe
+insertar a la base de datos, se 
+manejo directamente desde la 
+base y no por la aplicación.</t>
   </si>
 </sst>
 </file>
@@ -117,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -131,6 +230,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,8 +628,679 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="1"/>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="1">
+        <v>3</v>
+      </c>
+      <c r="H4" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="1">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="1">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="1">
+        <v>6</v>
+      </c>
+      <c r="H8" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="1">
+        <v>10</v>
+      </c>
+      <c r="H9" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="1">
+        <v>10</v>
+      </c>
+      <c r="H10" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>